<commit_message>
Projet final contenant le rapport, remis pour correction le 24/05/2018 par Dugauquier Rémy et Gille Madeleine
</commit_message>
<xml_diff>
--- a/Data/ecophysio2018/pc/ep2018_para.xlsx
+++ b/Data/ecophysio2018/pc/ep2018_para.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remydugauquier/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remydugauquier/VirtualBox VMs/svBox2017/Shared/Projects/ecophysio2018/Data/ecophysio2018/pc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B3294FE-BC29-7345-AD9D-A4F318D8F0DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4E4E1A-ADE9-3F46-8E85-0391457D9AFC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="940" windowWidth="24540" windowHeight="13660" xr2:uid="{8B5F76AF-5BE9-F94E-BEF5-BBCC99195C2A}"/>
+    <workbookView xWindow="720" yWindow="880" windowWidth="24540" windowHeight="13660" xr2:uid="{8B5F76AF-5BE9-F94E-BEF5-BBCC99195C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <t>2018-04-27 10:00:00</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>number_respiro</t>
   </si>
   <si>
@@ -166,6 +160,12 @@
   </si>
   <si>
     <t>35.3</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>LI</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:Q13"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,13 +544,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -558,16 +558,16 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -576,7 +576,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -587,13 +587,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -602,7 +602,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -613,13 +613,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -628,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -636,16 +636,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -654,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -665,13 +665,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -680,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="2"/>
@@ -694,13 +694,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -709,7 +709,7 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
@@ -720,16 +720,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -738,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="2"/>
@@ -749,16 +749,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -767,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="2"/>
@@ -778,16 +778,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -796,7 +796,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="2"/>
@@ -807,16 +807,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -825,7 +825,7 @@
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="2"/>
@@ -836,13 +836,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -854,7 +854,7 @@
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="2"/>
@@ -865,16 +865,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -883,7 +883,7 @@
         <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="2"/>
@@ -894,16 +894,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -912,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -920,16 +920,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -938,7 +938,7 @@
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -946,16 +946,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
         <v>39</v>
-      </c>
-      <c r="E16" t="s">
-        <v>41</v>
       </c>
       <c r="F16">
         <v>7</v>
@@ -964,7 +964,7 @@
         <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -972,16 +972,16 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>